<commit_message>
Run causality tests on our tris
</commit_message>
<xml_diff>
--- a/output/likelihood_formulas_M2.xlsx
+++ b/output/likelihood_formulas_M2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Individual</t>
   </si>
@@ -52,43 +52,52 @@
     <t>BXD1</t>
   </si>
   <si>
+    <t>BXD5</t>
+  </si>
+  <si>
+    <t>BXD31</t>
+  </si>
+  <si>
+    <t>BXD23</t>
+  </si>
+  <si>
+    <t>BXD2</t>
+  </si>
+  <si>
+    <t>BXD21</t>
+  </si>
+  <si>
     <t>BXD14</t>
   </si>
   <si>
-    <t>BXD2</t>
-  </si>
-  <si>
-    <t>BXD21</t>
-  </si>
-  <si>
-    <t>BXD23</t>
-  </si>
-  <si>
-    <t>BXD31</t>
+    <t>BXD13</t>
+  </si>
+  <si>
+    <t>BXD19</t>
+  </si>
+  <si>
+    <t>BXD15</t>
+  </si>
+  <si>
+    <t>BXD8</t>
+  </si>
+  <si>
+    <t>BXD24</t>
+  </si>
+  <si>
+    <t>BXD28</t>
+  </si>
+  <si>
+    <t>BXD32</t>
   </si>
   <si>
     <t>BXD11</t>
   </si>
   <si>
-    <t>BXD15</t>
+    <t>BXD6</t>
   </si>
   <si>
     <t>BXD16</t>
-  </si>
-  <si>
-    <t>BXD24</t>
-  </si>
-  <si>
-    <t>BXD28</t>
-  </si>
-  <si>
-    <t>BXD32</t>
-  </si>
-  <si>
-    <t>BXD6</t>
-  </si>
-  <si>
-    <t>BXD8</t>
   </si>
   <si>
     <t>BXD9</t>
@@ -449,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,36 +510,36 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.027</v>
+        <v>3.1855</v>
       </c>
       <c r="E2">
-        <v>5.3</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>3.183333333333334</v>
+        <v>38.875</v>
       </c>
       <c r="G2">
-        <v>1.338055555555555</v>
+        <v>1245.109375</v>
       </c>
       <c r="H2">
-        <v>1.266146835245512</v>
+        <v>2.99170483610721</v>
       </c>
       <c r="I2">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J2">
-        <v>0.06465291590195688</v>
+        <v>0.006162279433048035</v>
       </c>
       <c r="K2">
-        <v>0.7510578991915623</v>
+        <v>0.8007830544265581</v>
       </c>
       <c r="L2">
-        <v>0.02427904159696624</v>
+        <v>0.002467324473313082</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -539,36 +548,36 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.239</v>
+        <v>3.0645</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="F3">
-        <v>3.183333333333334</v>
+        <v>38.875</v>
       </c>
       <c r="G3">
-        <v>1.338055555555555</v>
+        <v>1245.109375</v>
       </c>
       <c r="H3">
-        <v>1.438804582540721</v>
+        <v>3.277132813667195</v>
       </c>
       <c r="I3">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J3">
-        <v>0.2688050773771029</v>
+        <v>0.005173048256839504</v>
       </c>
       <c r="K3">
-        <v>0.78158932586104</v>
+        <v>0.7861111914692198</v>
       </c>
       <c r="L3">
-        <v>0.1050475896075973</v>
+        <v>0.002033295564355937</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -577,36 +586,36 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1.166</v>
+        <v>2.931</v>
       </c>
       <c r="E4">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="F4">
-        <v>3.183333333333334</v>
+        <v>38.875</v>
       </c>
       <c r="G4">
-        <v>1.338055555555555</v>
+        <v>1245.109375</v>
       </c>
       <c r="H4">
-        <v>1.638025060189038</v>
+        <v>3.060482662025279</v>
       </c>
       <c r="I4">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J4">
-        <v>0.2896640519617951</v>
+        <v>0.00979881462615984</v>
       </c>
       <c r="K4">
-        <v>0.5125226083978361</v>
+        <v>0.8420217944128214</v>
       </c>
       <c r="L4">
-        <v>0.07422968773527278</v>
+        <v>0.004125407737318855</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -615,36 +624,36 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.9089999999999999</v>
+        <v>2.6615</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F5">
-        <v>3.183333333333334</v>
+        <v>38.875</v>
       </c>
       <c r="G5">
-        <v>1.338055555555555</v>
+        <v>1245.109375</v>
       </c>
       <c r="H5">
-        <v>1.571618234306266</v>
+        <v>3.060482662025279</v>
       </c>
       <c r="I5">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J5">
-        <v>0.3405794120351475</v>
+        <v>0.00979881462615984</v>
       </c>
       <c r="K5">
-        <v>0.3111778354464314</v>
+        <v>0.5969401540119526</v>
       </c>
       <c r="L5">
-        <v>0.05299038211735774</v>
+        <v>0.002924652956037214</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -653,36 +662,36 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.1865</v>
+        <v>3.2065</v>
       </c>
       <c r="E6">
-        <v>2.5</v>
+        <v>10</v>
       </c>
       <c r="F6">
-        <v>3.183333333333334</v>
+        <v>38.875</v>
       </c>
       <c r="G6">
-        <v>1.338055555555555</v>
+        <v>1245.109375</v>
       </c>
       <c r="H6">
-        <v>1.638025060189038</v>
+        <v>3.026093749066245</v>
       </c>
       <c r="I6">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J6">
-        <v>0.2896640519617951</v>
+        <v>0.008089049222233136</v>
       </c>
       <c r="K6">
-        <v>0.5354083298243082</v>
+        <v>0.8105321716427392</v>
       </c>
       <c r="L6">
-        <v>0.07754427313550316</v>
+        <v>0.003278217316310817</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -691,112 +700,112 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1.89</v>
+        <v>2.374</v>
       </c>
       <c r="E7">
-        <v>1.8</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>3.183333333333334</v>
+        <v>38.875</v>
       </c>
       <c r="G7">
-        <v>1.338055555555555</v>
+        <v>1245.109375</v>
       </c>
       <c r="H7">
-        <v>1.73099461642492</v>
+        <v>3.026093749066245</v>
       </c>
       <c r="I7">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J7">
-        <v>0.1687024282500931</v>
+        <v>0.008089049222233136</v>
       </c>
       <c r="K7">
-        <v>0.8084407205555387</v>
+        <v>0.3139567474823901</v>
       </c>
       <c r="L7">
-        <v>0.06819295632698717</v>
+        <v>0.001269805792018636</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>2.171</v>
+        <v>2.6955</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="F8">
-        <v>3.638888888888889</v>
+        <v>38.875</v>
       </c>
       <c r="G8">
-        <v>1.517098765432099</v>
+        <v>1245.109375</v>
       </c>
       <c r="H8">
-        <v>1.305990930775175</v>
+        <v>3.297766161442615</v>
       </c>
       <c r="I8">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J8">
-        <v>0.1758859568782206</v>
+        <v>0.004122144904925831</v>
       </c>
       <c r="K8">
-        <v>0.1524715479054494</v>
+        <v>0.3651159762517838</v>
       </c>
       <c r="L8">
-        <v>0.01340880205002671</v>
+        <v>0.0007525304806066557</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.8415</v>
+        <v>3.9685</v>
       </c>
       <c r="E9">
-        <v>2.9</v>
+        <v>79</v>
       </c>
       <c r="F9">
-        <v>3.638888888888889</v>
+        <v>38.875</v>
       </c>
       <c r="G9">
-        <v>1.517098765432099</v>
+        <v>1245.109375</v>
       </c>
       <c r="H9">
-        <v>1.58489959948282</v>
+        <v>3.263377248483581</v>
       </c>
       <c r="I9">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J9">
-        <v>0.2705568796570144</v>
+        <v>0.005922695085047902</v>
       </c>
       <c r="K9">
-        <v>0.7362120005072895</v>
+        <v>0.2638609740989317</v>
       </c>
       <c r="L9">
-        <v>0.09959361081165026</v>
+        <v>0.0007813840472158472</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -805,36 +814,36 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>1.031</v>
+        <v>2.905</v>
       </c>
       <c r="E10">
-        <v>2.95</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G10">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H10">
-        <v>1.578258916894543</v>
+        <v>2.99170483610721</v>
       </c>
       <c r="I10">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J10">
-        <v>0.2769980447648336</v>
+        <v>0.005338685304373844</v>
       </c>
       <c r="K10">
-        <v>0.4294069895091945</v>
+        <v>0.8610413921187994</v>
       </c>
       <c r="L10">
-        <v>0.05947244825120014</v>
+        <v>0.002298414513281115</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
@@ -843,36 +852,36 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>1.742</v>
+        <v>3.3835</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="F11">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G11">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H11">
-        <v>1.571618234306266</v>
+        <v>3.335593965697553</v>
       </c>
       <c r="I11">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J11">
-        <v>0.2831256128309231</v>
+        <v>0.004200626402036855</v>
       </c>
       <c r="K11">
-        <v>0.8014808763750364</v>
+        <v>0.871971737309845</v>
       </c>
       <c r="L11">
-        <v>0.1134598821479738</v>
+        <v>0.00183141375078684</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -881,36 +890,36 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>2.302</v>
+        <v>3.353</v>
       </c>
       <c r="E12">
-        <v>1.7</v>
+        <v>100</v>
       </c>
       <c r="F12">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G12">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H12">
-        <v>1.744275981601474</v>
+        <v>3.335593965697553</v>
       </c>
       <c r="I12">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J12">
-        <v>0.0938261323161729</v>
+        <v>0.004200626402036855</v>
       </c>
       <c r="K12">
-        <v>0.4181011246514542</v>
+        <v>0.8761771652902894</v>
       </c>
       <c r="L12">
-        <v>0.01961440572154402</v>
+        <v>0.0018402464666901</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -919,36 +928,36 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>1.2415</v>
+        <v>2.995</v>
       </c>
       <c r="E13">
-        <v>4.9</v>
+        <v>100</v>
       </c>
       <c r="F13">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G13">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H13">
-        <v>1.31927229595173</v>
+        <v>3.335593965697553</v>
       </c>
       <c r="I13">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J13">
-        <v>0.1917625863465881</v>
+        <v>0.004200626402036855</v>
       </c>
       <c r="K13">
-        <v>0.8451276423576342</v>
+        <v>0.6625633254156288</v>
       </c>
       <c r="L13">
-        <v>0.08103193124574712</v>
+        <v>0.001391590498881113</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="1">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
@@ -957,36 +966,36 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>1.07</v>
+        <v>4.2805</v>
       </c>
       <c r="E14">
-        <v>4.25</v>
+        <v>66</v>
       </c>
       <c r="F14">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G14">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H14">
-        <v>1.405601169599334</v>
+        <v>3.218671661636836</v>
       </c>
       <c r="I14">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J14">
-        <v>0.2863842059988284</v>
+        <v>0.008077451998695988</v>
       </c>
       <c r="K14">
-        <v>0.6608780899792053</v>
+        <v>0.05757624069766825</v>
       </c>
       <c r="L14">
-        <v>0.09463252353035848</v>
+        <v>0.0002325346602503909</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="1">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
@@ -995,36 +1004,36 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>2.446</v>
+        <v>3.072</v>
       </c>
       <c r="E15">
-        <v>2.55</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G15">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H15">
-        <v>1.631384377600761</v>
+        <v>2.99170483610721</v>
       </c>
       <c r="I15">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J15">
-        <v>0.2191255786365801</v>
+        <v>0.005338685304373844</v>
       </c>
       <c r="K15">
-        <v>0.1853560074436751</v>
+        <v>0.8632703772916952</v>
       </c>
       <c r="L15">
-        <v>0.02030812119243078</v>
+        <v>0.002304364438474218</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="1">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
@@ -1033,31 +1042,145 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>1.402</v>
+        <v>3.607</v>
       </c>
       <c r="E16">
-        <v>5.5</v>
+        <v>12</v>
       </c>
       <c r="F16">
-        <v>3.638888888888889</v>
+        <v>45.3</v>
       </c>
       <c r="G16">
-        <v>1.517098765432099</v>
+        <v>1960.41</v>
       </c>
       <c r="H16">
-        <v>1.239584104892403</v>
+        <v>3.032971531658052</v>
       </c>
       <c r="I16">
-        <v>0.216697217897322</v>
+        <v>0.2070144549413103</v>
       </c>
       <c r="J16">
-        <v>0.1034255012828138</v>
+        <v>0.006790613889094571</v>
       </c>
       <c r="K16">
-        <v>0.8063984660251935</v>
+        <v>0.3956147791747662</v>
       </c>
       <c r="L16">
-        <v>0.04170108279117386</v>
+        <v>0.001343233607097624</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3.387</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>45.3</v>
+      </c>
+      <c r="G17">
+        <v>1960.41</v>
+      </c>
+      <c r="H17">
+        <v>2.99170483610721</v>
+      </c>
+      <c r="I17">
+        <v>0.2070144549413103</v>
+      </c>
+      <c r="J17">
+        <v>0.005338685304373844</v>
+      </c>
+      <c r="K17">
+        <v>0.6011779633041984</v>
+      </c>
+      <c r="L17">
+        <v>0.001604749979002761</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>2.4065</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>45.3</v>
+      </c>
+      <c r="G18">
+        <v>1960.41</v>
+      </c>
+      <c r="H18">
+        <v>2.99170483610721</v>
+      </c>
+      <c r="I18">
+        <v>0.2070144549413103</v>
+      </c>
+      <c r="J18">
+        <v>0.005338685304373844</v>
+      </c>
+      <c r="K18">
+        <v>0.3834266793074632</v>
+      </c>
+      <c r="L18">
+        <v>0.001023497189061808</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3.0015</v>
+      </c>
+      <c r="E19">
+        <v>75</v>
+      </c>
+      <c r="F19">
+        <v>45.3</v>
+      </c>
+      <c r="G19">
+        <v>1960.41</v>
+      </c>
+      <c r="H19">
+        <v>3.249621683299968</v>
+      </c>
+      <c r="I19">
+        <v>0.2070144549413103</v>
+      </c>
+      <c r="J19">
+        <v>0.007195000363549942</v>
+      </c>
+      <c r="K19">
+        <v>0.7556696055810315</v>
+      </c>
+      <c r="L19">
+        <v>0.002718521543439581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>